<commit_message>
got rbf comparable to nn
</commit_message>
<xml_diff>
--- a/results_regression.xlsx
+++ b/results_regression.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierlim/R_Projects/KE5206NN/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pierl\OneDrive\Documents\R_Projects\KE5206NN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{ED98D36B-2772-1346-81DB-B6438E0546C9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="10_ncr:8100000_{ED98D36B-2772-1346-81DB-B6438E0546C9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="32" xr10:uidLastSave="{D6F9349E-B917-49C3-BB40-8690250AB28C}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" xr2:uid="{823390AE-0667-794E-9EC6-43A4D975E296}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>rmse (on test data)</t>
   </si>
@@ -67,13 +67,19 @@
   </si>
   <si>
     <t>But the predicted values are all the same!</t>
+  </si>
+  <si>
+    <t>rbf(size=8, rbfweights)
+rbf(nn_df, nn_df$shares, size=8, linOut=TRUE,
+                 initFunc = "RBF_Weights", initFuncParams = c(0.5, 0.5, 0.5, 0.5, 0.5, 0.5, 0.5, 0.5),
+                 learnFunc = "RadialBasisLearning", learnFuncParams = c(1e-05, 1e-05, 1e-05, 1e-05, 1e-05, 1e-05, 1e-05,1e-05))</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -97,6 +103,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -118,10 +138,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,20 +464,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{474D4A4B-B956-574B-9D6E-EF6B3FB2C243}">
   <dimension ref="A2:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="116" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="33" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.625" customWidth="1"/>
+    <col min="3" max="3" width="25.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -468,7 +495,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -488,7 +515,7 @@
         <v>1.100748E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -508,7 +535,7 @@
         <v>1.912316E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="79.5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
@@ -518,11 +545,14 @@
       <c r="D8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -536,10 +566,13 @@
         <v>6.6486749999999997E-2</v>
       </c>
       <c r="E9">
+        <v>2.419791E-2</v>
+      </c>
+      <c r="F9">
         <v>5.3307140000000003E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -549,20 +582,23 @@
       <c r="C10">
         <v>9.4380450000000005E-2</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>6.7679400000000001E-2</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="4">
+        <v>2.6383509999999999E-2</v>
+      </c>
+      <c r="F10">
         <v>5.443916E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E11" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>